<commit_message>
Add date formats, composite set
</commit_message>
<xml_diff>
--- a/test/files/style.xlsx
+++ b/test/files/style.xlsx
@@ -48,7 +48,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -70,7 +70,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF22FF00"/>
+        <fgColor rgb="99BB66"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAA000"/>
       </patternFill>
     </fill>
   </fills>
@@ -88,13 +98,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="0" horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -438,7 +450,9 @@
       <c r="J3"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4"/>
+      <c r="A4" s="4">
+        <v>39904.166666666664</v>
+      </c>
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4"/>
@@ -450,7 +464,9 @@
       <c r="J4"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5"/>
+      <c r="A5" s="5">
+        <v>39904.166666666664</v>
+      </c>
       <c r="B5"/>
       <c r="C5"/>
       <c r="D5"/>

</xml_diff>